<commit_message>
[Feat] - Added discount column
</commit_message>
<xml_diff>
--- a/webscraping_steam_test/2023_11_07_extract.xlsx
+++ b/webscraping_steam_test/2023_11_07_extract.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,11 @@
           <t>price_currency</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>discount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -523,6 +528,9 @@
           <t>R$</t>
         </is>
       </c>
+      <c r="K2" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -567,6 +575,9 @@
           <t>R$</t>
         </is>
       </c>
+      <c r="K3" t="n">
+        <v>50.01</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -611,6 +622,9 @@
           <t>R$</t>
         </is>
       </c>
+      <c r="K4" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -655,6 +669,9 @@
           <t>R$</t>
         </is>
       </c>
+      <c r="K5" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -699,6 +716,9 @@
           <t>R$</t>
         </is>
       </c>
+      <c r="K6" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -743,6 +763,9 @@
           <t>R$</t>
         </is>
       </c>
+      <c r="K7" t="n">
+        <v>84</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -750,42 +773,45 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Far Cry® 6</t>
+          <t>Overcooked! 2</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://cdn.cloudflare.steamstatic.com/steam/apps/2369390/header.jpg?t=1697654297</t>
+          <t>https://cdn.cloudflare.steamstatic.com/steam/apps/728880/header.jpg?t=1670442579</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>['Open World', 'FPS', 'Action', 'Adventure', 'Shooter']</t>
+          <t>['Multiplayer', 'Online Co-Op', 'Local Co-Op', 'Co-op', 'Casual']</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-05-11</t>
+          <t>2018-08-07</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>10601</v>
+        <v>38673</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Mixed</t>
+          <t>Very Positive</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>62.49</v>
+        <v>14.97</v>
       </c>
       <c r="I8" t="n">
-        <v>249.99</v>
+        <v>59.9</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
           <t>R$</t>
         </is>
+      </c>
+      <c r="K8" t="n">
+        <v>75.01000000000001</v>
       </c>
     </row>
     <row r="9">
@@ -794,42 +820,45 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Overcooked! 2</t>
+          <t>Far Cry® 6</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://cdn.cloudflare.steamstatic.com/steam/apps/728880/header.jpg?t=1670442579</t>
+          <t>https://cdn.cloudflare.steamstatic.com/steam/apps/2369390/header.jpg?t=1697654297</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>['Multiplayer', 'Online Co-Op', 'Local Co-Op', 'Co-op', 'Casual']</t>
+          <t>['Open World', 'FPS', 'Action', 'Adventure', 'Shooter']</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2018-08-07</t>
+          <t>2023-05-11</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>38673</v>
+        <v>10601</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Very Positive</t>
+          <t>Mixed</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>14.97</v>
+        <v>62.49</v>
       </c>
       <c r="I9" t="n">
-        <v>59.9</v>
+        <v>249.99</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
           <t>R$</t>
         </is>
+      </c>
+      <c r="K9" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="10">
@@ -838,26 +867,26 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Sniper Elite 4</t>
+          <t>Blasphemous</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://cdn.cloudflare.steamstatic.com/steam/apps/312660/header.jpg?t=1681207252</t>
+          <t>https://cdn.cloudflare.steamstatic.com/steam/apps/774361/header.jpg?t=1694433820</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>['Sniper', 'Action', 'Multiplayer', 'Shooter', 'War']</t>
+          <t>['Metroidvania', 'Pixel Graphics', 'Souls-like', 'Gore', 'Dark Fantasy']</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2017-02-13</t>
+          <t>2019-09-10</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>44272</v>
+        <v>28661</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -865,15 +894,18 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>10.59</v>
+        <v>33.47</v>
       </c>
       <c r="I10" t="n">
-        <v>105.99</v>
+        <v>133.9</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
           <t>R$</t>
         </is>
+      </c>
+      <c r="K10" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="11">
@@ -882,26 +914,26 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Blasphemous</t>
+          <t>Sniper Elite 4</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://cdn.cloudflare.steamstatic.com/steam/apps/774361/header.jpg?t=1694433820</t>
+          <t>https://cdn.cloudflare.steamstatic.com/steam/apps/312660/header.jpg?t=1681207252</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>['Metroidvania', 'Pixel Graphics', 'Souls-like', 'Gore', 'Dark Fantasy']</t>
+          <t>['Sniper', 'Action', 'Multiplayer', 'Shooter', 'War']</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2019-09-10</t>
+          <t>2017-02-13</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>28661</v>
+        <v>44272</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -909,15 +941,18 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>33.47</v>
+        <v>10.59</v>
       </c>
       <c r="I11" t="n">
-        <v>133.9</v>
+        <v>105.99</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
           <t>R$</t>
         </is>
+      </c>
+      <c r="K11" t="n">
+        <v>90.01000000000001</v>
       </c>
     </row>
     <row r="12">
@@ -961,6 +996,9 @@
           <t>R$</t>
         </is>
       </c>
+      <c r="K12" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1004,6 +1042,9 @@
         <is>
           <t>R$</t>
         </is>
+      </c>
+      <c r="K13" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>